<commit_message>
add correctly date reading
</commit_message>
<xml_diff>
--- a/listMinus.xlsx
+++ b/listMinus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinstahr/Repos/listComparator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8483A41A-03EC-3F43-A67E-7330817C6B21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF1B793-50AC-8146-8330-B6795562E98E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="940" windowWidth="25040" windowHeight="14220" xr2:uid="{2EFD0EC4-8BC1-6647-8D27-B0E594477E77}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
create prototype for compare lists
</commit_message>
<xml_diff>
--- a/listMinus.xlsx
+++ b/listMinus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinstahr/Repos/listComparator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\listComparator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF1B793-50AC-8146-8330-B6795562E98E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB31505-3976-4CCC-B0C6-8F888AE11D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="940" windowWidth="25040" windowHeight="14220" xr2:uid="{2EFD0EC4-8BC1-6647-8D27-B0E594477E77}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2EFD0EC4-8BC1-6647-8D27-B0E594477E77}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Datum</t>
   </si>
   <si>
     <t>Betrag</t>
+  </si>
+  <si>
+    <t>Belegnr.</t>
   </si>
 </sst>
 </file>
@@ -384,79 +387,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEF274C-BBCA-7443-A7EC-58738570D9F5}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43189</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
+        <v>6000001</v>
+      </c>
+      <c r="C2" s="1">
         <v>-3000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43189</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
+        <v>6000002</v>
+      </c>
+      <c r="C3" s="1">
         <v>-2830.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43189</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
+        <v>6000003</v>
+      </c>
+      <c r="C4" s="1">
         <v>-3600.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43187</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
+        <v>6000004</v>
+      </c>
+      <c r="C5" s="1">
         <v>-1000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43187</v>
       </c>
-      <c r="B6" s="1">
-        <v>-390</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>6000008</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-390.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43186</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
+        <v>6000006</v>
+      </c>
+      <c r="C7" s="1">
         <v>-27.3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43181</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
+        <v>6000010</v>
+      </c>
+      <c r="C8" s="1">
         <v>-140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>43160</v>
+      </c>
+      <c r="B9">
+        <v>6000011</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-250</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>